<commit_message>
fixed some minor bugs
</commit_message>
<xml_diff>
--- a/asset/questions.xlsx
+++ b/asset/questions.xlsx
@@ -4,12 +4,12 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="communication"/>
     <sheet r:id="rId2" sheetId="2" name="driving"/>
-    <sheet r:id="rId3" sheetId="3" name="laggage &amp;amp;amp; passenger"/>
+    <sheet r:id="rId3" sheetId="3" name="laggage &amp;amp;amp;amp; passenger"/>
     <sheet r:id="rId4" sheetId="4" name="yeguzo mereja"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
@@ -1487,7 +1487,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1504,12 +1504,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1556,7 +1550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1582,13 +1576,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1895,7 +1883,7 @@
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1910,28 +1898,28 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2989,7 +2977,7 @@
   </sheetPr>
   <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3003,33 +2991,33 @@
     <col min="8" max="8" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.2">
-      <c r="A1" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3049,7 +3037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3069,7 +3057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3089,7 +3077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3109,7 +3097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3129,7 +3117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3149,7 +3137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3169,7 +3157,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3189,7 +3177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3209,7 +3197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3229,7 +3217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3249,7 +3237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3269,7 +3257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.2">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3289,7 +3277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3309,7 +3297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3329,7 +3317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.4">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3349,7 +3337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3369,7 +3357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="15">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3389,7 +3377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3409,7 +3397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3429,7 +3417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>

</xml_diff>